<commit_message>
Latest changes on My account page
</commit_message>
<xml_diff>
--- a/KBL-Business flow/target/Data/Kbl datas.xlsx
+++ b/KBL-Business flow/target/Data/Kbl datas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>S.No</t>
   </si>
@@ -25,28 +25,79 @@
     <t>Shipping forms detail</t>
   </si>
   <si>
+    <t>Footer Links</t>
+  </si>
+  <si>
+    <t>Categeory</t>
+  </si>
+  <si>
     <t>testautomatin@gmail.com</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
+    <t>CONTACT US</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL</t>
+  </si>
+  <si>
     <t>Test@0605</t>
   </si>
   <si>
     <t>Enter</t>
   </si>
   <si>
+    <t>1800-123-4443</t>
+  </si>
+  <si>
+    <t>COMMERCIAL</t>
+  </si>
+  <si>
     <t>TNT Garments</t>
   </si>
   <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>INDUSTRY</t>
+  </si>
+  <si>
     <t>Thillai area</t>
   </si>
   <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>AGRICULTURAL</t>
+  </si>
+  <si>
     <t>SAF Games Village</t>
   </si>
   <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>SERVICES</t>
+  </si>
+  <si>
     <t>Sri Sakthi Nagar</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>SELECT YOUR PUMP</t>
+  </si>
+  <si>
+    <t>Installation/Inspection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privacy Policy for Website </t>
+  </si>
+  <si>
+    <t>My Wishlist</t>
   </si>
 </sst>
 </file>
@@ -116,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -124,7 +175,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -139,17 +190,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -157,8 +202,17 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -465,20 +519,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="29.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,92 +543,143 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="10"/>
-      <c r="B5" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="10"/>
-      <c r="B7" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="9">
         <v>110001</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="11">
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="9">
         <v>6383762492</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>